<commit_message>
fixed issue with newsday pdf
</commit_message>
<xml_diff>
--- a/Exp 3.xlsx
+++ b/Exp 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Parth/Desktop/College/CSM/Practical/CSM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{08F8C3E9-0563-7D41-AB53-5AB9ACA165DA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B4A368CD-D931-6346-A7B5-D61AD12647C9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" activeTab="2" xr2:uid="{8BE2681C-6454-3842-9C37-454C8C74535F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" activeTab="1" xr2:uid="{8BE2681C-6454-3842-9C37-454C8C74535F}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch C" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>Probability</t>
   </si>
@@ -174,6 +174,9 @@
   <si>
     <t>Processing time for jobs are normally distributed with mean 50 minutes and standard deviation 8 minutes. 
 Construct a simulation table, and perform a simulation for 20 new customers. Assume that when the simulation begins there is one job being processed (scheduled to be completed in 25 minutes) and there is one job with 50 minutes processing time in the queue</t>
+  </si>
+  <si>
+    <t>R(IAT)</t>
   </si>
 </sst>
 </file>
@@ -229,10 +232,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -557,7 +560,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,10 +602,10 @@
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4"/>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5"/>
       <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
@@ -612,10 +615,10 @@
       <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="4"/>
+      <c r="M2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3">
@@ -688,7 +691,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="5"/>
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -897,7 +900,7 @@
       </c>
       <c r="L13">
         <f ca="1">RAND()</f>
-        <v>0.87925079753283597</v>
+        <v>0.26741816033352639</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -940,7 +943,7 @@
       </c>
       <c r="L14">
         <f t="shared" ref="L14:L23" ca="1" si="6">RAND()</f>
-        <v>0.61296179145380725</v>
+        <v>0.27705583663382605</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -983,7 +986,7 @@
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="6"/>
-        <v>0.58093272337290536</v>
+        <v>0.41605343664402028</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1026,7 +1029,7 @@
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="6"/>
-        <v>0.58427363839121538</v>
+        <v>5.7729710220772779E-2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1037,7 +1040,7 @@
         <v>0.19373955833646839</v>
       </c>
       <c r="C17">
-        <f>IF(B17&lt;=$G$3,$C$3,IF(B17&lt;=$G$4,$C$4,IF(B17&lt;=$G$5,$C$5,IF(B17&lt;=$H9,$C$6,IF(B17&lt;=$G$7,$C$7,$C$8)))))</f>
+        <f t="shared" ref="C17:C23" si="9">IF(B17&lt;=$G$3,$C$3,IF(B17&lt;=$G$4,$C$4,IF(B17&lt;=$G$5,$C$5,IF(B17&lt;=$H9,$C$6,IF(B17&lt;=$G$7,$C$7,$C$8)))))</f>
         <v>1</v>
       </c>
       <c r="D17">
@@ -1069,7 +1072,7 @@
       </c>
       <c r="L17">
         <f t="shared" ca="1" si="6"/>
-        <v>0.75851512767316587</v>
+        <v>0.12259215566339343</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1080,7 +1083,7 @@
         <v>0.36697107791682759</v>
       </c>
       <c r="C18">
-        <f>IF(B18&lt;=$G$3,$C$3,IF(B18&lt;=$G$4,$C$4,IF(B18&lt;=$G$5,$C$5,IF(B18&lt;=$H10,$C$6,IF(B18&lt;=$G$7,$C$7,$C$8)))))</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="D18">
@@ -1112,7 +1115,7 @@
       </c>
       <c r="L18">
         <f t="shared" ca="1" si="6"/>
-        <v>0.11932631794988602</v>
+        <v>0.56618326031037114</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1123,7 +1126,7 @@
         <v>0.52857441618120793</v>
       </c>
       <c r="C19">
-        <f>IF(B19&lt;=$G$3,$C$3,IF(B19&lt;=$G$4,$C$4,IF(B19&lt;=$G$5,$C$5,IF(B19&lt;=$H11,$C$6,IF(B19&lt;=$G$7,$C$7,$C$8)))))</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="D19">
@@ -1155,7 +1158,7 @@
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="6"/>
-        <v>0.63432926280633162</v>
+        <v>0.84438631971553457</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1166,7 +1169,7 @@
         <v>0.55114231752271325</v>
       </c>
       <c r="C20">
-        <f>IF(B20&lt;=$G$3,$C$3,IF(B20&lt;=$G$4,$C$4,IF(B20&lt;=$G$5,$C$5,IF(B20&lt;=$H12,$C$6,IF(B20&lt;=$G$7,$C$7,$C$8)))))</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="D20">
@@ -1198,7 +1201,7 @@
       </c>
       <c r="L20">
         <f t="shared" ca="1" si="6"/>
-        <v>0.28617030943481792</v>
+        <v>0.4893114758791538</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1209,7 +1212,7 @@
         <v>0.71835910001485792</v>
       </c>
       <c r="C21">
-        <f>IF(B21&lt;=$G$3,$C$3,IF(B21&lt;=$G$4,$C$4,IF(B21&lt;=$G$5,$C$5,IF(B21&lt;=$H13,$C$6,IF(B21&lt;=$G$7,$C$7,$C$8)))))</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="D21">
@@ -1241,7 +1244,7 @@
       </c>
       <c r="L21">
         <f t="shared" ca="1" si="6"/>
-        <v>0.21840879167949123</v>
+        <v>0.52844454399549079</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1252,7 +1255,7 @@
         <v>0.16653934156475281</v>
       </c>
       <c r="C22">
-        <f>IF(B22&lt;=$G$3,$C$3,IF(B22&lt;=$G$4,$C$4,IF(B22&lt;=$G$5,$C$5,IF(B22&lt;=$H14,$C$6,IF(B22&lt;=$G$7,$C$7,$C$8)))))</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="D22">
@@ -1284,7 +1287,7 @@
       </c>
       <c r="L22">
         <f t="shared" ca="1" si="6"/>
-        <v>0.94269656560198467</v>
+        <v>0.77322081484488914</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1295,7 +1298,7 @@
         <v>0.8710824368006358</v>
       </c>
       <c r="C23">
-        <f>IF(B23&lt;=$G$3,$C$3,IF(B23&lt;=$G$4,$C$4,IF(B23&lt;=$G$5,$C$5,IF(B23&lt;=$H15,$C$6,IF(B23&lt;=$G$7,$C$7,$C$8)))))</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="D23">
@@ -1327,7 +1330,7 @@
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="6"/>
-        <v>0.90252062783520559</v>
+        <v>0.99842586132908406</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1357,932 +1360,1012 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7271F4-F163-6643-892D-D8FC6E7045BA}">
-  <dimension ref="A4:K42"/>
+  <dimension ref="A4:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C5">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0.45</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C6">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.15</v>
       </c>
-      <c r="D6">
-        <f>(C6+SUM(D5:D5))</f>
+      <c r="E6">
+        <f>(D6+SUM(E5:E5))</f>
         <v>0.6</v>
       </c>
-      <c r="E6">
-        <f>F5+0.01</f>
+      <c r="F6">
+        <f>G5+0.01</f>
         <v>0.46</v>
       </c>
-      <c r="F6">
-        <f>D6</f>
+      <c r="G6">
+        <f>E6</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>3</v>
-      </c>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
         <v>0.2</v>
       </c>
-      <c r="D7">
-        <f t="shared" ref="D7:D8" si="0">(C7+SUM(D6:D6))</f>
+      <c r="E7">
+        <f t="shared" ref="E7:E8" si="0">(D7+SUM(E6:E6))</f>
         <v>0.8</v>
       </c>
-      <c r="E7">
-        <f t="shared" ref="E7:E8" si="1">F6+0.01</f>
+      <c r="F7">
+        <f t="shared" ref="F7:F8" si="1">G6+0.01</f>
         <v>0.61</v>
       </c>
-      <c r="F7">
-        <f t="shared" ref="F7:F8" si="2">D7</f>
+      <c r="G7">
+        <f t="shared" ref="G7:G8" si="2">E7</f>
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C8">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.2</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <f t="shared" si="1"/>
         <v>0.81</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>19</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>8</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>9</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>10</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>20</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>21</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>0.22915196831887474</v>
       </c>
-      <c r="F12">
-        <f>IF(E12&lt;=$F$5,$B$5,IF(E12&lt;=$F$6,$B$6,IF(E12&lt;=$F$7,$B$7,$B$8)))</f>
-        <v>1</v>
-      </c>
       <c r="G12">
-        <v>0</v>
+        <f>IF(F12&lt;=$G$5,$C$5,IF(F12&lt;=$G$6,$C$6,IF(F12&lt;=$G$7,$C$7,$C$8)))</f>
+        <v>1</v>
       </c>
       <c r="H12">
-        <f>G12+F12</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <f>H12-D12</f>
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
+        <f>H12+G12</f>
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <f>I12-E12</f>
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
         <v>13</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13">
+        <f t="shared" ref="C13:C31" ca="1" si="3">RANDBETWEEN(1,6)</f>
+        <v>3</v>
+      </c>
+      <c r="D13">
         <v>5</v>
       </c>
-      <c r="D13">
-        <f>D12+C13</f>
+      <c r="E13">
+        <f>E12+D13</f>
         <v>5</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>0.79806332003262026</v>
       </c>
-      <c r="F13">
-        <f t="shared" ref="F13:F31" si="3">IF(E13&lt;=$F$5,$B$5,IF(E13&lt;=$F$6,$B$6,IF(E13&lt;=$F$7,$B$7,$B$8)))</f>
-        <v>3</v>
-      </c>
       <c r="G13">
-        <f>MAX(H12,D13)</f>
+        <f t="shared" ref="G13:G31" si="4">IF(F13&lt;=$G$5,$C$5,IF(F13&lt;=$G$6,$C$6,IF(F13&lt;=$G$7,$C$7,$C$8)))</f>
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <f>MAX(I12,E13)</f>
         <v>5</v>
       </c>
-      <c r="H13">
-        <f>G13+F13</f>
+      <c r="I13">
+        <f>H13+G13</f>
         <v>8</v>
       </c>
-      <c r="I13">
-        <f t="shared" ref="I13:I31" si="4">H13-D13</f>
-        <v>3</v>
-      </c>
       <c r="J13">
-        <f>G13-H12</f>
+        <f t="shared" ref="J13:J31" si="5">I13-E13</f>
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <f>H13-I12</f>
         <v>4</v>
       </c>
-      <c r="K13">
-        <f>G13-D13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <f>H13-E13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D14">
         <v>4</v>
       </c>
-      <c r="D14">
-        <f t="shared" ref="D14:D31" si="5">D13+C14</f>
+      <c r="E14">
+        <f t="shared" ref="E14:E31" si="6">E13+D14</f>
         <v>9</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>0.14756879157301916</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
       <c r="G14">
-        <f t="shared" ref="G14:G31" si="6">MAX(H13,D14)</f>
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H31" si="7">MAX(I13,E14)</f>
         <v>9</v>
       </c>
-      <c r="H14">
-        <f t="shared" ref="H14:H31" si="7">G14+F14</f>
+      <c r="I14">
+        <f t="shared" ref="I14:I31" si="8">H14+G14</f>
         <v>10</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="J14">
-        <f t="shared" ref="J14:J31" si="8">G14-H13</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="K14">
-        <f t="shared" ref="K14:K31" si="9">G14-D14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+        <f t="shared" ref="K14:K31" si="9">H14-I13</f>
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L31" si="10">H14-E14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>4</v>
       </c>
       <c r="C15">
+        <f t="shared" ca="1" si="3"/>
         <v>4</v>
       </c>
       <c r="D15">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>0.4919806335525404</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G15">
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="7"/>
-        <v>15</v>
-      </c>
-      <c r="I15">
+      <c r="F15">
+        <v>0.4919806335525404</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
+      <c r="H15">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
       <c r="J15">
-        <f t="shared" si="8"/>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="K15">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>5</v>
       </c>
       <c r="C16">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
       <c r="E16">
-        <v>0.19614764052809186</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G16">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
+      <c r="F16">
+        <v>0.19614764052809186</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="H16">
         <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="J16">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="K16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>6</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
       </c>
       <c r="D17">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>0.74510870075830171</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="G17">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
+      <c r="F17">
+        <v>0.74510870075830171</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
       <c r="H17">
         <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
       <c r="J17">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="K17">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>7</v>
       </c>
       <c r="C18">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D18">
         <v>2</v>
       </c>
-      <c r="D18">
+      <c r="E18">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>0.93772584934680214</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="7"/>
+        <v>21</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="J18">
         <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-      <c r="E18">
-        <v>0.93772584934680214</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="H18">
+      <c r="F19">
+        <v>0.17891860103720836</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="7"/>
         <v>25</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="4"/>
+      <c r="I19">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
         <v>5</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19">
-        <v>8</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="5"/>
-        <v>21</v>
-      </c>
-      <c r="E19">
-        <v>0.17891860103720836</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="6"/>
-        <v>25</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="7"/>
-        <v>26</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="8"/>
-        <v>0</v>
       </c>
       <c r="K19">
         <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>9</v>
       </c>
       <c r="C20">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="D20">
         <v>6</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="5"/>
-        <v>27</v>
-      </c>
       <c r="E20">
-        <v>0.73063051951605307</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="G20">
         <f t="shared" si="6"/>
         <v>27</v>
       </c>
+      <c r="F20">
+        <v>0.73063051951605307</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
       <c r="H20">
         <f t="shared" si="7"/>
+        <v>27</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
       <c r="J20">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="K20">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>10</v>
       </c>
       <c r="C21">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D21">
         <v>5</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="5"/>
-        <v>32</v>
-      </c>
       <c r="E21">
-        <v>0.95784073278610071</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="G21">
         <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="7"/>
-        <v>36</v>
-      </c>
-      <c r="I21">
+      <c r="F21">
+        <v>0.95784073278610071</v>
+      </c>
+      <c r="G21">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
+      <c r="H21">
+        <f t="shared" si="7"/>
+        <v>32</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
       <c r="J21">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="K21">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>11</v>
       </c>
       <c r="C22">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D22">
         <v>5</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="5"/>
-        <v>37</v>
-      </c>
       <c r="E22">
-        <v>0.9372349295892124</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="G22">
         <f t="shared" si="6"/>
         <v>37</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="7"/>
-        <v>41</v>
-      </c>
-      <c r="I22">
+      <c r="F22">
+        <v>0.9372349295892124</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
+      <c r="H22">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="8"/>
+        <v>41</v>
+      </c>
       <c r="J22">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="K22">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>12</v>
       </c>
       <c r="C23">
+        <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
       <c r="D23">
-        <f t="shared" si="5"/>
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="E23">
-        <v>0.3458257466553859</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G23">
         <f t="shared" si="6"/>
         <v>43</v>
       </c>
+      <c r="F23">
+        <v>0.3458257466553859</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="H23">
         <f t="shared" si="7"/>
+        <v>43</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="8"/>
         <v>44</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="J23">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="K23">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>13</v>
       </c>
       <c r="C24">
+        <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
       <c r="D24">
-        <f t="shared" si="5"/>
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E24">
-        <v>0.28872422353618288</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G24">
         <f t="shared" si="6"/>
         <v>46</v>
       </c>
+      <c r="F24">
+        <v>0.28872422353618288</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="H24">
         <f t="shared" si="7"/>
+        <v>46</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="8"/>
         <v>47</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="J24">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="K24">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>14</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
       </c>
       <c r="D25">
-        <f t="shared" si="5"/>
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="E25">
-        <v>0.88878434693206587</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="G25">
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="H25">
-        <f t="shared" si="7"/>
-        <v>53</v>
-      </c>
-      <c r="I25">
+      <c r="F25">
+        <v>0.88878434693206587</v>
+      </c>
+      <c r="G25">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
+      <c r="H25">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="8"/>
+        <v>53</v>
+      </c>
       <c r="J25">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="K25">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>15</v>
       </c>
       <c r="C26">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="5"/>
-        <v>54</v>
-      </c>
       <c r="E26">
-        <v>5.7681613057262715E-2</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G26">
         <f t="shared" si="6"/>
         <v>54</v>
       </c>
+      <c r="F26">
+        <v>5.7681613057262715E-2</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="H26">
         <f t="shared" si="7"/>
+        <v>54</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="J26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="K26">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>16</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="D27">
-        <f t="shared" si="5"/>
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="E27">
-        <v>0.15804962490561769</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G27">
         <f t="shared" si="6"/>
         <v>57</v>
       </c>
+      <c r="F27">
+        <v>0.15804962490561769</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="H27">
         <f t="shared" si="7"/>
+        <v>57</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="8"/>
         <v>58</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="J27">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="K27">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>17</v>
       </c>
       <c r="C28">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D28">
         <v>5</v>
       </c>
-      <c r="D28">
-        <f t="shared" si="5"/>
-        <v>62</v>
-      </c>
       <c r="E28">
-        <v>0.40282022264997774</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G28">
         <f t="shared" si="6"/>
         <v>62</v>
       </c>
+      <c r="F28">
+        <v>0.40282022264997774</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="H28">
         <f t="shared" si="7"/>
+        <v>62</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="J28">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="K28">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>18</v>
       </c>
       <c r="C29">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D29">
         <v>4</v>
       </c>
-      <c r="D29">
-        <f t="shared" si="5"/>
-        <v>66</v>
-      </c>
       <c r="E29">
-        <v>8.4984220020738577E-2</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G29">
         <f t="shared" si="6"/>
         <v>66</v>
       </c>
+      <c r="F29">
+        <v>8.4984220020738577E-2</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="H29">
         <f t="shared" si="7"/>
+        <v>66</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="8"/>
         <v>67</v>
       </c>
-      <c r="I29">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="J29">
-        <f t="shared" si="8"/>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="K29">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>19</v>
       </c>
       <c r="C30">
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D30">
-        <f t="shared" si="5"/>
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>0.16028303298945556</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G30">
         <f t="shared" si="6"/>
         <v>67</v>
       </c>
+      <c r="F30">
+        <v>0.16028303298945556</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="H30">
         <f t="shared" si="7"/>
+        <v>67</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="8"/>
         <v>68</v>
       </c>
-      <c r="I30">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="J30">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="K30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>20</v>
       </c>
       <c r="C31">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="D31">
         <v>6</v>
       </c>
-      <c r="D31">
-        <f t="shared" si="5"/>
-        <v>73</v>
-      </c>
       <c r="E31">
-        <v>0.43266367087256874</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G31">
         <f t="shared" si="6"/>
         <v>73</v>
       </c>
+      <c r="F31">
+        <v>0.43266367087256874</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
       <c r="H31">
         <f t="shared" si="7"/>
+        <v>73</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="8"/>
         <v>74</v>
       </c>
-      <c r="I31">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="J31">
-        <f t="shared" si="8"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="K31">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H32" t="s">
+        <v>5</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
         <v>23</v>
       </c>
-      <c r="I32">
-        <f>AVERAGE(I12:I31)</f>
+      <c r="J32">
+        <f>AVERAGE(J12:J31)</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="J32">
-        <f t="shared" ref="J32:K32" si="10">AVERAGE(J12:J31)</f>
+      <c r="K32">
+        <f t="shared" ref="K32:L32" si="11">AVERAGE(K12:K31)</f>
         <v>1.8421052631578947</v>
       </c>
-      <c r="K32">
-        <f t="shared" si="10"/>
+      <c r="L32">
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
     </row>
@@ -2291,7 +2374,7 @@
         <v>24</v>
       </c>
       <c r="B35">
-        <f>K32</f>
+        <f>L32</f>
         <v>0.25</v>
       </c>
     </row>
@@ -2300,7 +2383,7 @@
         <v>25</v>
       </c>
       <c r="B36">
-        <f>COUNTIF(K12:K31,"&lt;&gt;0")/COUNT(K12:K31)</f>
+        <f>COUNTIF(L12:L31,"&lt;&gt;0")/COUNT(L12:L31)</f>
         <v>0.1</v>
       </c>
     </row>
@@ -2309,7 +2392,7 @@
         <v>26</v>
       </c>
       <c r="B37">
-        <f>SUM(K12:K31)/COUNTIF(K12:K31,"&lt;&gt;0")</f>
+        <f>SUM(L12:L31)/COUNTIF(L12:L31,"&lt;&gt;0")</f>
         <v>2.5</v>
       </c>
     </row>
@@ -2318,7 +2401,7 @@
         <v>27</v>
       </c>
       <c r="B38">
-        <f>J32</f>
+        <f>K32</f>
         <v>1.8421052631578947</v>
       </c>
     </row>
@@ -2327,7 +2410,7 @@
         <v>28</v>
       </c>
       <c r="B39">
-        <f>AVERAGE(F12:F31)</f>
+        <f>AVERAGE(G12:G31)</f>
         <v>1.95</v>
       </c>
     </row>
@@ -2336,7 +2419,7 @@
         <v>29</v>
       </c>
       <c r="B40">
-        <f>B5*C5+B6*C6+B7*C7+B8*C8</f>
+        <f>C5*D5+C6*D6+C7*D7+C8*D8</f>
         <v>2.1500000000000004</v>
       </c>
     </row>
@@ -2345,7 +2428,7 @@
         <v>30</v>
       </c>
       <c r="B41">
-        <f>AVERAGE(C12:C31)</f>
+        <f>AVERAGE(D12:D31)</f>
         <v>3.65</v>
       </c>
     </row>
@@ -2354,13 +2437,13 @@
         <v>31</v>
       </c>
       <c r="B42">
-        <f>AVERAGE(MAX(C12:C31),MIN(C12:C31))</f>
+        <f>AVERAGE(MAX(D12:D31),MIN(D12:D31))</f>
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2370,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA44E87-B67F-F344-BF28-0F81A2C5A942}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2595,11 +2678,11 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <f>H12+G12</f>
+        <f t="shared" ref="I12:I22" si="3">H12+G12</f>
         <v>0.42</v>
       </c>
       <c r="J12">
-        <f>I12-E12</f>
+        <f t="shared" ref="J12:J22" si="4">I12-E12</f>
         <v>0.42</v>
       </c>
       <c r="K12">
@@ -2630,15 +2713,15 @@
         <v>0.83</v>
       </c>
       <c r="H13">
-        <f>MAX(I12,E13)</f>
+        <f t="shared" ref="H13:H22" si="5">MAX(I12,E13)</f>
         <v>0.42</v>
       </c>
       <c r="I13">
-        <f>H13+G13</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="J13">
-        <f>I13-E13</f>
+        <f t="shared" si="4"/>
         <v>1.25</v>
       </c>
       <c r="K13">
@@ -2646,7 +2729,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <f>H13-E13</f>
+        <f t="shared" ref="L13:L22" si="6">H13-E13</f>
         <v>0.42</v>
       </c>
     </row>
@@ -2658,38 +2741,38 @@
         <v>0.14756879157301916</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D13:D33" si="3">IF(C14&lt;=$G$5,$B$5,IF(C14&lt;=$G$6,$B$6,IF(C14&lt;=$G$7,$B$7,$B$8)))</f>
+        <f t="shared" ref="D14:D33" si="7">IF(C14&lt;=$G$5,$B$5,IF(C14&lt;=$G$6,$B$6,IF(C14&lt;=$G$7,$B$7,$B$8)))</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f t="shared" ref="E14:E33" si="4">E13+D14</f>
+        <f t="shared" ref="E14:E33" si="8">E13+D14</f>
         <v>0</v>
       </c>
       <c r="F14">
         <v>0.14756879157301916</v>
       </c>
       <c r="G14">
-        <f>ROUND(NORMINV(F14,$I$6,$J$6),2)</f>
+        <f t="shared" ref="G14:G22" si="9">ROUND(NORMINV(F14,$I$6,$J$6),2)</f>
         <v>0.69</v>
       </c>
       <c r="H14">
-        <f>MAX(I13,E14)</f>
+        <f t="shared" si="5"/>
         <v>1.25</v>
       </c>
       <c r="I14">
-        <f>H14+G14</f>
+        <f t="shared" si="3"/>
         <v>1.94</v>
       </c>
       <c r="J14">
-        <f>I14-E14</f>
+        <f t="shared" si="4"/>
         <v>1.94</v>
       </c>
       <c r="K14">
-        <f t="shared" ref="K14:K31" si="5">H14-I13</f>
+        <f t="shared" ref="K14:K22" si="10">H14-I13</f>
         <v>0</v>
       </c>
       <c r="L14">
-        <f>H14-E14</f>
+        <f t="shared" si="6"/>
         <v>1.25</v>
       </c>
     </row>
@@ -2701,38 +2784,38 @@
         <v>0.4919806335525404</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F15">
         <v>0.4919806335525404</v>
       </c>
       <c r="G15">
-        <f>ROUND(NORMINV(F15,$I$6,$J$6),2)</f>
+        <f t="shared" si="9"/>
         <v>0.83</v>
       </c>
       <c r="H15">
-        <f>MAX(I14,E15)</f>
+        <f t="shared" si="5"/>
         <v>1.94</v>
       </c>
       <c r="I15">
-        <f>H15+G15</f>
+        <f t="shared" si="3"/>
         <v>2.77</v>
       </c>
       <c r="J15">
-        <f>I15-E15</f>
+        <f t="shared" si="4"/>
         <v>1.77</v>
       </c>
       <c r="K15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L15">
-        <f>H15-E15</f>
+        <f t="shared" si="6"/>
         <v>0.94</v>
       </c>
     </row>
@@ -2744,38 +2827,38 @@
         <v>0.19614764052809186</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F16">
         <v>0.19614764052809186</v>
       </c>
       <c r="G16">
-        <f>ROUND(NORMINV(F16,$I$6,$J$6),2)</f>
+        <f t="shared" si="9"/>
         <v>0.72</v>
       </c>
       <c r="H16">
-        <f>MAX(I15,E16)</f>
+        <f t="shared" si="5"/>
         <v>2.77</v>
       </c>
       <c r="I16">
-        <f>H16+G16</f>
+        <f t="shared" si="3"/>
         <v>3.49</v>
       </c>
       <c r="J16">
-        <f>I16-E16</f>
+        <f t="shared" si="4"/>
         <v>2.4900000000000002</v>
       </c>
       <c r="K16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L16">
-        <f>H16-E16</f>
+        <f t="shared" si="6"/>
         <v>1.77</v>
       </c>
     </row>
@@ -2787,38 +2870,38 @@
         <v>0.74510870075830171</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="F17">
         <v>0.74510870075830171</v>
       </c>
       <c r="G17">
-        <f>ROUND(NORMINV(F17,$I$6,$J$6),2)</f>
+        <f t="shared" si="9"/>
         <v>0.92</v>
       </c>
       <c r="H17">
-        <f>MAX(I16,E17)</f>
+        <f t="shared" si="5"/>
         <v>3.49</v>
       </c>
       <c r="I17">
-        <f>H17+G17</f>
+        <f t="shared" si="3"/>
         <v>4.41</v>
       </c>
       <c r="J17">
-        <f>I17-E17</f>
+        <f t="shared" si="4"/>
         <v>1.4100000000000001</v>
       </c>
       <c r="K17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L17">
-        <f>H17-E17</f>
+        <f t="shared" si="6"/>
         <v>0.49000000000000021</v>
       </c>
     </row>
@@ -2830,38 +2913,38 @@
         <v>0.93772584934680214</v>
       </c>
       <c r="D18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="E18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="F18">
         <v>0.93772584934680214</v>
       </c>
       <c r="G18">
-        <f>ROUND(NORMINV(F18,$I$6,$J$6),2)</f>
+        <f t="shared" si="9"/>
         <v>1.03</v>
       </c>
       <c r="H18">
-        <f>MAX(I17,E18)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I18">
-        <f>H18+G18</f>
+        <f t="shared" si="3"/>
         <v>7.03</v>
       </c>
       <c r="J18">
-        <f>I18-E18</f>
+        <f t="shared" si="4"/>
         <v>1.0300000000000002</v>
       </c>
       <c r="K18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1.5899999999999999</v>
       </c>
       <c r="L18">
-        <f>H18-E18</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2873,38 +2956,38 @@
         <v>0.17891860103720836</v>
       </c>
       <c r="D19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="F19">
         <v>0.17891860103720836</v>
       </c>
       <c r="G19">
-        <f>ROUND(NORMINV(F19,$I$6,$J$6),2)</f>
+        <f t="shared" si="9"/>
         <v>0.71</v>
       </c>
       <c r="H19">
-        <f>MAX(I18,E19)</f>
+        <f t="shared" si="5"/>
         <v>7.03</v>
       </c>
       <c r="I19">
-        <f>H19+G19</f>
+        <f t="shared" si="3"/>
         <v>7.74</v>
       </c>
       <c r="J19">
-        <f>I19-E19</f>
+        <f t="shared" si="4"/>
         <v>1.7400000000000002</v>
       </c>
       <c r="K19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L19">
-        <f>H19-E19</f>
+        <f t="shared" si="6"/>
         <v>1.0300000000000002</v>
       </c>
     </row>
@@ -2916,38 +2999,38 @@
         <v>0.73063051951605307</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="F20">
         <v>0.73063051951605307</v>
       </c>
       <c r="G20">
-        <f>ROUND(NORMINV(F20,$I$6,$J$6),2)</f>
+        <f t="shared" si="9"/>
         <v>0.91</v>
       </c>
       <c r="H20">
-        <f>MAX(I19,E20)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I20">
-        <f>H20+G20</f>
+        <f t="shared" si="3"/>
         <v>8.91</v>
       </c>
       <c r="J20">
-        <f>I20-E20</f>
+        <f t="shared" si="4"/>
         <v>0.91000000000000014</v>
       </c>
       <c r="K20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.25999999999999979</v>
       </c>
       <c r="L20">
-        <f>H20-E20</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2959,38 +3042,38 @@
         <v>0.95784073278610071</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="E21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="F21">
         <v>0.95784073278610071</v>
       </c>
       <c r="G21">
-        <f>ROUND(NORMINV(F21,$I$6,$J$6),2)</f>
+        <f t="shared" si="9"/>
         <v>1.05</v>
       </c>
       <c r="H21">
-        <f>MAX(I20,E21)</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="I21">
-        <f>H21+G21</f>
+        <f t="shared" si="3"/>
         <v>12.05</v>
       </c>
       <c r="J21">
-        <f>I21-E21</f>
+        <f t="shared" si="4"/>
         <v>1.0500000000000007</v>
       </c>
       <c r="K21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.09</v>
       </c>
       <c r="L21">
-        <f>H21-E21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3002,38 +3085,38 @@
         <v>0.9372349295892124</v>
       </c>
       <c r="D22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="E22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="F22">
         <v>0.9372349295892124</v>
       </c>
       <c r="G22">
-        <f>ROUND(NORMINV(F22,$I$6,$J$6),2)</f>
+        <f t="shared" si="9"/>
         <v>1.03</v>
       </c>
       <c r="H22">
-        <f>MAX(I21,E22)</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="I22">
-        <f>H22+G22</f>
+        <f t="shared" si="3"/>
         <v>15.03</v>
       </c>
       <c r="J22">
-        <f>I22-E22</f>
+        <f t="shared" si="4"/>
         <v>1.0299999999999994</v>
       </c>
       <c r="K22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1.9499999999999993</v>
       </c>
       <c r="L22">
-        <f>H22-E22</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3045,38 +3128,38 @@
         <v>0.85505757567041518</v>
       </c>
       <c r="D23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="F23">
         <v>0.33986830248044475</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:G33" si="6">ROUND(NORMINV(F23,$I$6,$J$6),2)</f>
+        <f t="shared" ref="G23:G33" si="11">ROUND(NORMINV(F23,$I$6,$J$6),2)</f>
         <v>0.78</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:H33" si="7">MAX(I22,E23)</f>
+        <f t="shared" ref="H23:H33" si="12">MAX(I22,E23)</f>
         <v>16</v>
       </c>
       <c r="I23">
-        <f t="shared" ref="I23:I33" si="8">H23+G23</f>
+        <f t="shared" ref="I23:I33" si="13">H23+G23</f>
         <v>16.78</v>
       </c>
       <c r="J23">
-        <f t="shared" ref="J23:J33" si="9">I23-E23</f>
+        <f t="shared" ref="J23:J33" si="14">I23-E23</f>
         <v>0.78000000000000114</v>
       </c>
       <c r="K23">
-        <f t="shared" ref="K23:K33" si="10">H23-I22</f>
+        <f t="shared" ref="K23:K33" si="15">H23-I22</f>
         <v>0.97000000000000064</v>
       </c>
       <c r="L23">
-        <f t="shared" ref="L23:L33" si="11">H23-E23</f>
+        <f t="shared" ref="L23:L33" si="16">H23-E23</f>
         <v>0</v>
       </c>
     </row>
@@ -3088,38 +3171,38 @@
         <v>7.3091854574403703E-2</v>
       </c>
       <c r="D24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="F24">
         <v>0.49077706852442937</v>
       </c>
       <c r="G24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.83</v>
       </c>
       <c r="H24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>16.78</v>
       </c>
       <c r="I24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>17.61</v>
       </c>
       <c r="J24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>1.6099999999999994</v>
       </c>
       <c r="K24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0.78000000000000114</v>
       </c>
     </row>
@@ -3131,38 +3214,38 @@
         <v>2.8331029843627564E-2</v>
       </c>
       <c r="D25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="F25">
         <v>0.48913038497004646</v>
       </c>
       <c r="G25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.83</v>
       </c>
       <c r="H25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>17.61</v>
       </c>
       <c r="I25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>18.439999999999998</v>
       </c>
       <c r="J25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>2.4399999999999977</v>
       </c>
       <c r="K25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.6099999999999994</v>
       </c>
     </row>
@@ -3174,38 +3257,38 @@
         <v>3.6244144562430636E-2</v>
       </c>
       <c r="D26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="F26">
         <v>0.19928593131488825</v>
       </c>
       <c r="G26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.72</v>
       </c>
       <c r="H26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>18.439999999999998</v>
       </c>
       <c r="I26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>19.159999999999997</v>
       </c>
       <c r="J26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.1599999999999966</v>
       </c>
       <c r="K26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.4399999999999977</v>
       </c>
     </row>
@@ -3217,38 +3300,38 @@
         <v>0.82927984801678956</v>
       </c>
       <c r="D27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="F27">
         <v>0.32651302023916906</v>
       </c>
       <c r="G27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.77</v>
       </c>
       <c r="H27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>19.159999999999997</v>
       </c>
       <c r="I27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>19.929999999999996</v>
       </c>
       <c r="J27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>1.9299999999999962</v>
       </c>
       <c r="K27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.1599999999999966</v>
       </c>
     </row>
@@ -3260,38 +3343,38 @@
         <v>0.20201076791389583</v>
       </c>
       <c r="D28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="F28">
         <v>0.34288876823286052</v>
       </c>
       <c r="G28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.78</v>
       </c>
       <c r="H28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>19.929999999999996</v>
       </c>
       <c r="I28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>20.709999999999997</v>
       </c>
       <c r="J28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>2.7099999999999973</v>
       </c>
       <c r="K28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.9299999999999962</v>
       </c>
     </row>
@@ -3303,38 +3386,38 @@
         <v>0.10033541082193909</v>
       </c>
       <c r="D29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="F29">
         <v>0.52144619245948842</v>
       </c>
       <c r="G29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.84</v>
       </c>
       <c r="H29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>20.709999999999997</v>
       </c>
       <c r="I29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>21.549999999999997</v>
       </c>
       <c r="J29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.5499999999999972</v>
       </c>
       <c r="K29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.7099999999999973</v>
       </c>
     </row>
@@ -3346,38 +3429,38 @@
         <v>0.50147438623080642</v>
       </c>
       <c r="D30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="F30">
         <v>0.67646240183692974</v>
       </c>
       <c r="G30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.89</v>
       </c>
       <c r="H30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>21.549999999999997</v>
       </c>
       <c r="I30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>22.439999999999998</v>
       </c>
       <c r="J30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.4399999999999977</v>
       </c>
       <c r="K30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.5499999999999972</v>
       </c>
     </row>
@@ -3389,38 +3472,38 @@
         <v>0.52847610909746112</v>
       </c>
       <c r="D31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="F31">
         <v>0.45618218230058771</v>
       </c>
       <c r="G31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.82</v>
       </c>
       <c r="H31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>22.439999999999998</v>
       </c>
       <c r="I31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>23.259999999999998</v>
       </c>
       <c r="J31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.259999999999998</v>
       </c>
       <c r="K31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.4399999999999977</v>
       </c>
     </row>
@@ -3432,38 +3515,38 @@
         <v>0.39032895566927273</v>
       </c>
       <c r="D32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="E32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="F32">
         <v>0.79182375438243935</v>
       </c>
       <c r="G32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.94</v>
       </c>
       <c r="H32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>23.259999999999998</v>
       </c>
       <c r="I32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>24.2</v>
       </c>
       <c r="J32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.1999999999999993</v>
       </c>
       <c r="K32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>2.259999999999998</v>
       </c>
     </row>
@@ -3475,38 +3558,38 @@
         <v>0.82398045964411137</v>
       </c>
       <c r="D33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="E33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="F33">
         <v>0.96509812793607841</v>
       </c>
       <c r="G33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.07</v>
       </c>
       <c r="H33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>24.2</v>
       </c>
       <c r="I33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>25.27</v>
       </c>
       <c r="J33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>2.2699999999999996</v>
       </c>
       <c r="K33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>1.1999999999999993</v>
       </c>
     </row>

</xml_diff>